<commit_message>
Update notebooks with correct online profile and re-run reports notebook
</commit_message>
<xml_diff>
--- a/guide/12-enrich-data-with-thematic-information/reports/esri_buffered_business_summary.xlsx
+++ b/guide/12-enrich-data-with-thematic-information/reports/esri_buffered_business_summary.xlsx
@@ -31,7 +31,7 @@
         <x:color rgb="FF00436D"/>
         <x:rFont val="Verdana"/>
       </x:rPr>
-      <x:t xml:space="preserve">Copyright 2021 Data Axle, Inc. All rights reserved. Esri Total Residential Population forecasts for 2021.</x:t>
+      <x:t xml:space="preserve">Copyright 2022 Data Axle, Inc. All rights reserved. Esri Total Residential Population forecasts for 2022.</x:t>
     </x:r>
     <x:r>
       <x:rPr>
@@ -125,7 +125,7 @@
         <x:color rgb="FF00436D"/>
         <x:rFont val="Verdana"/>
       </x:rPr>
-      <x:t xml:space="preserve">Copyright 2021 Data Axle, Inc. All rights reserved. Esri Total Residential Population forecasts for 2021.</x:t>
+      <x:t xml:space="preserve">Copyright 2022 Data Axle, Inc. All rights reserved. Esri Total Residential Population forecasts for 2022.</x:t>
     </x:r>
     <x:r>
       <x:rPr>
@@ -641,15 +641,15 @@
       </x:c>
       <x:c r="G10" s="10"/>
       <x:c r="L10" s="11" t="n">
-        <x:v>1569</x:v>
+        <x:v>1718</x:v>
       </x:c>
       <x:c r="AE10" s="10"/>
       <x:c r="AL10" s="11" t="n">
-        <x:v>1833</x:v>
+        <x:v>1887</x:v>
       </x:c>
       <x:c r="BE10" s="10"/>
       <x:c r="BK10" s="11" t="n">
-        <x:v>2190</x:v>
+        <x:v>2326</x:v>
       </x:c>
     </x:row>
     <x:row r="11" ht="10.95" customHeight="1">
@@ -658,15 +658,15 @@
       </x:c>
       <x:c r="G11" s="13"/>
       <x:c r="L11" s="14" t="n">
-        <x:v>20210</x:v>
+        <x:v>21383</x:v>
       </x:c>
       <x:c r="AE11" s="13"/>
       <x:c r="AL11" s="14" t="n">
-        <x:v>21860</x:v>
+        <x:v>22285</x:v>
       </x:c>
       <x:c r="BE11" s="13"/>
       <x:c r="BK11" s="14" t="n">
-        <x:v>43758</x:v>
+        <x:v>44836</x:v>
       </x:c>
     </x:row>
     <x:row r="12" ht="10.2" customHeight="1">
@@ -675,15 +675,15 @@
       </x:c>
       <x:c r="G12" s="10"/>
       <x:c r="L12" s="11" t="n">
-        <x:v>13185</x:v>
+        <x:v>13366</x:v>
       </x:c>
       <x:c r="AE12" s="10"/>
       <x:c r="AL12" s="11" t="n">
-        <x:v>63146</x:v>
+        <x:v>65217</x:v>
       </x:c>
       <x:c r="BE12" s="10"/>
       <x:c r="BK12" s="11" t="n">
-        <x:v>81315</x:v>
+        <x:v>83986</x:v>
       </x:c>
     </x:row>
     <x:row r="13" ht="10.2" customHeight="1">
@@ -692,15 +692,15 @@
       </x:c>
       <x:c r="G13" s="13"/>
       <x:c r="L13" s="14" t="n">
-        <x:v>153</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="AE13" s="13"/>
       <x:c r="AL13" s="14" t="n">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="BE13" s="13"/>
       <x:c r="BK13" s="14" t="n">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="14" ht="9.45" customHeight="1">
@@ -776,37 +776,37 @@
         <x:v>Agriculture &amp; Mining</x:v>
       </x:c>
       <x:c r="J16" s="17" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="Q16" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="W16" s="17" t="n">
-        <x:v>87</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="Z16" s="18" t="n">
-        <x:v>0.4</x:v>
+        <x:v>0.5</x:v>
       </x:c>
       <x:c r="AI16" s="17" t="n">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="AN16" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AU16" s="17" t="n">
-        <x:v>86</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="AY16" s="18" t="n">
-        <x:v>0.4</x:v>
+        <x:v>0.9</x:v>
       </x:c>
       <x:c r="BG16" s="17" t="n">
-        <x:v>27</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="BO16" s="18" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1.1</x:v>
       </x:c>
       <x:c r="BT16" s="17" t="n">
-        <x:v>242</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="BW16" s="18" t="n">
         <x:v>0.6</x:v>
@@ -817,37 +817,37 @@
         <x:v>Construction</x:v>
       </x:c>
       <x:c r="J17" s="20" t="n">
-        <x:v>81</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="Q17" s="21" t="n">
-        <x:v>5.2</x:v>
+        <x:v>4.9</x:v>
       </x:c>
       <x:c r="W17" s="20" t="n">
-        <x:v>571</x:v>
+        <x:v>461</x:v>
       </x:c>
       <x:c r="Z17" s="21" t="n">
-        <x:v>2.8</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="AI17" s="20" t="n">
-        <x:v>106</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="AN17" s="21" t="n">
         <x:v>5.8</x:v>
       </x:c>
       <x:c r="AU17" s="20" t="n">
-        <x:v>682</x:v>
+        <x:v>555</x:v>
       </x:c>
       <x:c r="AY17" s="21" t="n">
-        <x:v>3.1</x:v>
+        <x:v>2.5</x:v>
       </x:c>
       <x:c r="BG17" s="20" t="n">
-        <x:v>164</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="BO17" s="21" t="n">
-        <x:v>7.5</x:v>
+        <x:v>7.6</x:v>
       </x:c>
       <x:c r="BT17" s="20" t="n">
-        <x:v>1229</x:v>
+        <x:v>1266</x:v>
       </x:c>
       <x:c r="BW17" s="21" t="n">
         <x:v>2.8</x:v>
@@ -858,40 +858,40 @@
         <x:v>Manufacturing</x:v>
       </x:c>
       <x:c r="J18" s="17" t="n">
-        <x:v>35</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="Q18" s="18" t="n">
-        <x:v>2.2</x:v>
+        <x:v>2.3</x:v>
       </x:c>
       <x:c r="W18" s="17" t="n">
-        <x:v>316</x:v>
+        <x:v>389</x:v>
       </x:c>
       <x:c r="Z18" s="18" t="n">
-        <x:v>1.6</x:v>
+        <x:v>1.8</x:v>
       </x:c>
       <x:c r="AI18" s="17" t="n">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="AN18" s="18" t="n">
         <x:v>2.1</x:v>
       </x:c>
       <x:c r="AU18" s="17" t="n">
-        <x:v>563</x:v>
+        <x:v>676</x:v>
       </x:c>
       <x:c r="AY18" s="18" t="n">
-        <x:v>2.6</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="BG18" s="17" t="n">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="BO18" s="18" t="n">
+        <x:v>3.1</x:v>
+      </x:c>
+      <x:c r="BT18" s="17" t="n">
+        <x:v>1498</x:v>
+      </x:c>
+      <x:c r="BW18" s="18" t="n">
         <x:v>3.3</x:v>
-      </x:c>
-      <x:c r="BT18" s="17" t="n">
-        <x:v>1556</x:v>
-      </x:c>
-      <x:c r="BW18" s="18" t="n">
-        <x:v>3.6</x:v>
       </x:c>
     </x:row>
     <x:row r="19" ht="10.2" customHeight="1">
@@ -899,40 +899,40 @@
         <x:v>Transportation</x:v>
       </x:c>
       <x:c r="J19" s="20" t="n">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="Q19" s="21" t="n">
+        <x:v>1.3</x:v>
+      </x:c>
+      <x:c r="W19" s="20" t="n">
+        <x:v>307</x:v>
+      </x:c>
+      <x:c r="Z19" s="21" t="n">
+        <x:v>1.4</x:v>
+      </x:c>
+      <x:c r="AI19" s="20" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AN19" s="21" t="n">
+        <x:v>2.5</x:v>
+      </x:c>
+      <x:c r="AU19" s="20" t="n">
+        <x:v>660</x:v>
+      </x:c>
+      <x:c r="AY19" s="21" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="BG19" s="20" t="n">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="BO19" s="21" t="n">
+        <x:v>3.2</x:v>
+      </x:c>
+      <x:c r="BT19" s="20" t="n">
+        <x:v>503</x:v>
+      </x:c>
+      <x:c r="BW19" s="21" t="n">
         <x:v>1.1</x:v>
-      </x:c>
-      <x:c r="W19" s="20" t="n">
-        <x:v>161</x:v>
-      </x:c>
-      <x:c r="Z19" s="21" t="n">
-        <x:v>0.8</x:v>
-      </x:c>
-      <x:c r="AI19" s="20" t="n">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="AN19" s="21" t="n">
-        <x:v>2.2</x:v>
-      </x:c>
-      <x:c r="AU19" s="20" t="n">
-        <x:v>355</x:v>
-      </x:c>
-      <x:c r="AY19" s="21" t="n">
-        <x:v>1.6</x:v>
-      </x:c>
-      <x:c r="BG19" s="20" t="n">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="BO19" s="21" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="BT19" s="20" t="n">
-        <x:v>504</x:v>
-      </x:c>
-      <x:c r="BW19" s="21" t="n">
-        <x:v>1.2</x:v>
       </x:c>
     </x:row>
     <x:row r="20" ht="10.2" customHeight="1">
@@ -940,37 +940,37 @@
         <x:v>Communication</x:v>
       </x:c>
       <x:c r="J20" s="17" t="n">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="Q20" s="18" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.5</x:v>
       </x:c>
       <x:c r="W20" s="17" t="n">
-        <x:v>96</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="Z20" s="18" t="n">
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="AI20" s="17" t="n">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="AN20" s="18" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1.1</x:v>
       </x:c>
       <x:c r="AU20" s="17" t="n">
-        <x:v>328</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="AY20" s="18" t="n">
-        <x:v>1.5</x:v>
+        <x:v>1.4</x:v>
       </x:c>
       <x:c r="BG20" s="17" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="BO20" s="18" t="n">
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="BT20" s="17" t="n">
-        <x:v>82</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="BW20" s="18" t="n">
         <x:v>0.2</x:v>
@@ -984,13 +984,13 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="Q21" s="21" t="n">
-        <x:v>0.4</x:v>
+        <x:v>0.3</x:v>
       </x:c>
       <x:c r="W21" s="20" t="n">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="Z21" s="21" t="n">
-        <x:v>0.3</x:v>
+        <x:v>0.2</x:v>
       </x:c>
       <x:c r="AI21" s="20" t="n">
         <x:v>3</x:v>
@@ -999,10 +999,10 @@
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="AU21" s="20" t="n">
-        <x:v>100</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="AY21" s="21" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.4</x:v>
       </x:c>
       <x:c r="BG21" s="20" t="n">
         <x:v>7</x:v>
@@ -1011,10 +1011,10 @@
         <x:v>0.3</x:v>
       </x:c>
       <x:c r="BT21" s="20" t="n">
-        <x:v>285</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="BW21" s="21" t="n">
-        <x:v>0.7</x:v>
+        <x:v>0.3</x:v>
       </x:c>
     </x:row>
     <x:row r="22" ht="10.2" customHeight="1">
@@ -1022,40 +1022,40 @@
         <x:v>Wholesale Trade</x:v>
       </x:c>
       <x:c r="J22" s="17" t="n">
-        <x:v>33</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="Q22" s="18" t="n">
-        <x:v>2.1</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="W22" s="17" t="n">
-        <x:v>327</x:v>
+        <x:v>574</x:v>
       </x:c>
       <x:c r="Z22" s="18" t="n">
-        <x:v>1.6</x:v>
+        <x:v>2.7</x:v>
       </x:c>
       <x:c r="AI22" s="17" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="AN22" s="18" t="n">
         <x:v>1.9</x:v>
       </x:c>
       <x:c r="AU22" s="17" t="n">
-        <x:v>440</x:v>
+        <x:v>490</x:v>
       </x:c>
       <x:c r="AY22" s="18" t="n">
-        <x:v>2</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="BG22" s="17" t="n">
-        <x:v>79</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="BO22" s="18" t="n">
-        <x:v>3.6</x:v>
+        <x:v>3.5</x:v>
       </x:c>
       <x:c r="BT22" s="17" t="n">
-        <x:v>1304</x:v>
+        <x:v>1154</x:v>
       </x:c>
       <x:c r="BW22" s="18" t="n">
-        <x:v>3</x:v>
+        <x:v>2.6</x:v>
       </x:c>
     </x:row>
     <x:row r="23" ht="9.9" customHeight="1">
@@ -1078,40 +1078,40 @@
         <x:v>Retail Trade Summary</x:v>
       </x:c>
       <x:c r="J24" s="20" t="n">
-        <x:v>333</x:v>
+        <x:v>362</x:v>
       </x:c>
       <x:c r="Q24" s="21" t="n">
-        <x:v>21.2</x:v>
+        <x:v>21.1</x:v>
       </x:c>
       <x:c r="W24" s="20" t="n">
-        <x:v>4420</x:v>
+        <x:v>4835</x:v>
       </x:c>
       <x:c r="Z24" s="21" t="n">
-        <x:v>21.9</x:v>
+        <x:v>22.6</x:v>
       </x:c>
       <x:c r="AI24" s="20" t="n">
-        <x:v>359</x:v>
+        <x:v>356</x:v>
       </x:c>
       <x:c r="AN24" s="21" t="n">
-        <x:v>19.6</x:v>
+        <x:v>18.9</x:v>
       </x:c>
       <x:c r="AU24" s="20" t="n">
-        <x:v>8125</x:v>
+        <x:v>7846</x:v>
       </x:c>
       <x:c r="AY24" s="21" t="n">
-        <x:v>37.2</x:v>
+        <x:v>35.2</x:v>
       </x:c>
       <x:c r="BG24" s="20" t="n">
-        <x:v>439</x:v>
+        <x:v>449</x:v>
       </x:c>
       <x:c r="BO24" s="21" t="n">
-        <x:v>20</x:v>
+        <x:v>19.3</x:v>
       </x:c>
       <x:c r="BT24" s="20" t="n">
-        <x:v>8180</x:v>
+        <x:v>8356</x:v>
       </x:c>
       <x:c r="BW24" s="21" t="n">
-        <x:v>18.7</x:v>
+        <x:v>18.6</x:v>
       </x:c>
     </x:row>
     <x:row r="25" ht="10.2" customHeight="1">
@@ -1119,40 +1119,40 @@
         <x:v>Home Improvement</x:v>
       </x:c>
       <x:c r="J25" s="17" t="n">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="Q25" s="18" t="n">
         <x:v>0.9</x:v>
       </x:c>
       <x:c r="W25" s="17" t="n">
-        <x:v>490</x:v>
+        <x:v>418</x:v>
       </x:c>
       <x:c r="Z25" s="18" t="n">
-        <x:v>2.4</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="AI25" s="17" t="n">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="AN25" s="18" t="n">
         <x:v>0.8</x:v>
       </x:c>
       <x:c r="AU25" s="17" t="n">
-        <x:v>409</x:v>
+        <x:v>484</x:v>
       </x:c>
       <x:c r="AY25" s="18" t="n">
-        <x:v>1.9</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="BG25" s="17" t="n">
-        <x:v>34</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="BO25" s="18" t="n">
-        <x:v>1.6</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="BT25" s="17" t="n">
-        <x:v>601</x:v>
+        <x:v>513</x:v>
       </x:c>
       <x:c r="BW25" s="18" t="n">
-        <x:v>1.4</x:v>
+        <x:v>1.1</x:v>
       </x:c>
     </x:row>
     <x:row r="26" ht="10.2" customHeight="1">
@@ -1160,28 +1160,28 @@
         <x:v>General Merchandise Stores</x:v>
       </x:c>
       <x:c r="J26" s="20" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="Q26" s="21" t="n">
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="W26" s="20" t="n">
-        <x:v>128</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="Z26" s="21" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="AI26" s="20" t="n">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="AN26" s="21" t="n">
-        <x:v>1</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="AU26" s="20" t="n">
-        <x:v>762</x:v>
+        <x:v>711</x:v>
       </x:c>
       <x:c r="AY26" s="21" t="n">
-        <x:v>3.5</x:v>
+        <x:v>3.2</x:v>
       </x:c>
       <x:c r="BG26" s="20" t="n">
         <x:v>13</x:v>
@@ -1190,10 +1190,10 @@
         <x:v>0.6</x:v>
       </x:c>
       <x:c r="BT26" s="20" t="n">
-        <x:v>797</x:v>
+        <x:v>767</x:v>
       </x:c>
       <x:c r="BW26" s="21" t="n">
-        <x:v>1.8</x:v>
+        <x:v>1.7</x:v>
       </x:c>
     </x:row>
     <x:row r="27" ht="10.2" customHeight="1">
@@ -1201,40 +1201,40 @@
         <x:v>Food Stores</x:v>
       </x:c>
       <x:c r="J27" s="17" t="n">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="Q27" s="18" t="n">
-        <x:v>2</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="W27" s="17" t="n">
-        <x:v>533</x:v>
+        <x:v>582</x:v>
       </x:c>
       <x:c r="Z27" s="18" t="n">
-        <x:v>2.6</x:v>
+        <x:v>2.7</x:v>
       </x:c>
       <x:c r="AI27" s="17" t="n">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="AN27" s="18" t="n">
         <x:v>2.6</x:v>
       </x:c>
       <x:c r="AU27" s="17" t="n">
-        <x:v>841</x:v>
+        <x:v>902</x:v>
       </x:c>
       <x:c r="AY27" s="18" t="n">
-        <x:v>3.8</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="BG27" s="17" t="n">
-        <x:v>55</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="BO27" s="18" t="n">
         <x:v>2.5</x:v>
       </x:c>
       <x:c r="BT27" s="17" t="n">
-        <x:v>568</x:v>
+        <x:v>748</x:v>
       </x:c>
       <x:c r="BW27" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.7</x:v>
       </x:c>
     </x:row>
     <x:row r="28" ht="10.2" customHeight="1">
@@ -1242,40 +1242,40 @@
         <x:v>Auto Dealers, Gas Stations, Auto Aftermarket</x:v>
       </x:c>
       <x:c r="J28" s="20" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="Q28" s="21" t="n">
-        <x:v>2</x:v>
+        <x:v>1.9</x:v>
       </x:c>
       <x:c r="W28" s="20" t="n">
-        <x:v>543</x:v>
+        <x:v>615</x:v>
       </x:c>
       <x:c r="Z28" s="21" t="n">
-        <x:v>2.7</x:v>
+        <x:v>2.9</x:v>
       </x:c>
       <x:c r="AI28" s="20" t="n">
-        <x:v>25</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="AN28" s="21" t="n">
-        <x:v>1.4</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AU28" s="20" t="n">
-        <x:v>412</x:v>
+        <x:v>360</x:v>
       </x:c>
       <x:c r="AY28" s="21" t="n">
+        <x:v>1.6</x:v>
+      </x:c>
+      <x:c r="BG28" s="20" t="n">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="BO28" s="21" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="BT28" s="20" t="n">
+        <x:v>839</x:v>
+      </x:c>
+      <x:c r="BW28" s="21" t="n">
         <x:v>1.9</x:v>
-      </x:c>
-      <x:c r="BG28" s="20" t="n">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="BO28" s="21" t="n">
-        <x:v>3.3</x:v>
-      </x:c>
-      <x:c r="BT28" s="20" t="n">
-        <x:v>616</x:v>
-      </x:c>
-      <x:c r="BW28" s="21" t="n">
-        <x:v>1.4</x:v>
       </x:c>
     </x:row>
     <x:row r="29" ht="10.2" customHeight="1">
@@ -1283,37 +1283,37 @@
         <x:v>Apparel &amp; Accessory Stores</x:v>
       </x:c>
       <x:c r="J29" s="17" t="n">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="Q29" s="18" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="W29" s="17" t="n">
-        <x:v>131</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="Z29" s="18" t="n">
         <x:v>0.6</x:v>
       </x:c>
       <x:c r="AI29" s="17" t="n">
-        <x:v>19</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="AN29" s="18" t="n">
-        <x:v>1</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="AU29" s="17" t="n">
-        <x:v>287</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="AY29" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="BG29" s="17" t="n">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="BO29" s="18" t="n">
-        <x:v>0.3</x:v>
+        <x:v>0.2</x:v>
       </x:c>
       <x:c r="BT29" s="17" t="n">
-        <x:v>65</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="BW29" s="18" t="n">
         <x:v>0.1</x:v>
@@ -1324,40 +1324,40 @@
         <x:v>Furniture &amp; Home Furnishings</x:v>
       </x:c>
       <x:c r="J30" s="20" t="n">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="Q30" s="21" t="n">
-        <x:v>1.4</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="W30" s="20" t="n">
-        <x:v>116</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="Z30" s="21" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.7</x:v>
       </x:c>
       <x:c r="AI30" s="20" t="n">
-        <x:v>26</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="AN30" s="21" t="n">
-        <x:v>1.4</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="AU30" s="20" t="n">
-        <x:v>242</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="AY30" s="21" t="n">
-        <x:v>1.1</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="BG30" s="20" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="BO30" s="21" t="n">
         <x:v>1.2</x:v>
       </x:c>
       <x:c r="BT30" s="20" t="n">
-        <x:v>329</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="BW30" s="21" t="n">
-        <x:v>0.8</x:v>
+        <x:v>0.6</x:v>
       </x:c>
     </x:row>
     <x:row r="31" ht="10.2" customHeight="1">
@@ -1365,40 +1365,40 @@
         <x:v>Eating &amp; Drinking Places</x:v>
       </x:c>
       <x:c r="J31" s="17" t="n">
-        <x:v>120</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="Q31" s="18" t="n">
-        <x:v>7.6</x:v>
+        <x:v>7.8</x:v>
       </x:c>
       <x:c r="W31" s="17" t="n">
-        <x:v>1526</x:v>
+        <x:v>1588</x:v>
       </x:c>
       <x:c r="Z31" s="18" t="n">
-        <x:v>7.6</x:v>
+        <x:v>7.4</x:v>
       </x:c>
       <x:c r="AI31" s="17" t="n">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="AN31" s="18" t="n">
-        <x:v>6.8</x:v>
+        <x:v>6.7</x:v>
       </x:c>
       <x:c r="AU31" s="17" t="n">
-        <x:v>1951</x:v>
+        <x:v>1894</x:v>
       </x:c>
       <x:c r="AY31" s="18" t="n">
-        <x:v>8.9</x:v>
+        <x:v>8.5</x:v>
       </x:c>
       <x:c r="BG31" s="17" t="n">
-        <x:v>138</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="BO31" s="18" t="n">
-        <x:v>6.3</x:v>
+        <x:v>6.5</x:v>
       </x:c>
       <x:c r="BT31" s="17" t="n">
-        <x:v>2436</x:v>
+        <x:v>2535</x:v>
       </x:c>
       <x:c r="BW31" s="18" t="n">
-        <x:v>5.6</x:v>
+        <x:v>5.7</x:v>
       </x:c>
     </x:row>
     <x:row r="32" ht="10.2" customHeight="1">
@@ -1406,40 +1406,40 @@
         <x:v>Miscellaneous Retail</x:v>
       </x:c>
       <x:c r="J32" s="20" t="n">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="Q32" s="21" t="n">
-        <x:v>5.8</x:v>
+        <x:v>5.4</x:v>
       </x:c>
       <x:c r="W32" s="20" t="n">
-        <x:v>953</x:v>
+        <x:v>1187</x:v>
       </x:c>
       <x:c r="Z32" s="21" t="n">
-        <x:v>4.7</x:v>
+        <x:v>5.6</x:v>
       </x:c>
       <x:c r="AI32" s="20" t="n">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="AN32" s="21" t="n">
         <x:v>4.7</x:v>
       </x:c>
       <x:c r="AU32" s="20" t="n">
-        <x:v>3223</x:v>
+        <x:v>3091</x:v>
       </x:c>
       <x:c r="AY32" s="21" t="n">
-        <x:v>14.7</x:v>
+        <x:v>13.9</x:v>
       </x:c>
       <x:c r="BG32" s="20" t="n">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="BO32" s="21" t="n">
-        <x:v>4.2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="BT32" s="20" t="n">
-        <x:v>2769</x:v>
+        <x:v>2609</x:v>
       </x:c>
       <x:c r="BW32" s="21" t="n">
-        <x:v>6.3</x:v>
+        <x:v>5.8</x:v>
       </x:c>
     </x:row>
     <x:row r="33" ht="9.9" customHeight="1">
@@ -1462,40 +1462,40 @@
         <x:v>Finance, Insurance, Real Estate Summary</x:v>
       </x:c>
       <x:c r="J34" s="20" t="n">
-        <x:v>164</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="Q34" s="21" t="n">
-        <x:v>10.5</x:v>
+        <x:v>10.9</x:v>
       </x:c>
       <x:c r="W34" s="20" t="n">
-        <x:v>1006</x:v>
+        <x:v>1107</x:v>
       </x:c>
       <x:c r="Z34" s="21" t="n">
+        <x:v>5.2</x:v>
+      </x:c>
+      <x:c r="AI34" s="20" t="n">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="AN34" s="21" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="AU34" s="20" t="n">
+        <x:v>1233</x:v>
+      </x:c>
+      <x:c r="AY34" s="21" t="n">
+        <x:v>5.5</x:v>
+      </x:c>
+      <x:c r="BG34" s="20" t="n">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="BO34" s="21" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="BT34" s="20" t="n">
+        <x:v>2253</x:v>
+      </x:c>
+      <x:c r="BW34" s="21" t="n">
         <x:v>5</x:v>
-      </x:c>
-      <x:c r="AI34" s="20" t="n">
-        <x:v>192</x:v>
-      </x:c>
-      <x:c r="AN34" s="21" t="n">
-        <x:v>10.5</x:v>
-      </x:c>
-      <x:c r="AU34" s="20" t="n">
-        <x:v>1258</x:v>
-      </x:c>
-      <x:c r="AY34" s="21" t="n">
-        <x:v>5.8</x:v>
-      </x:c>
-      <x:c r="BG34" s="20" t="n">
-        <x:v>167</x:v>
-      </x:c>
-      <x:c r="BO34" s="21" t="n">
-        <x:v>7.6</x:v>
-      </x:c>
-      <x:c r="BT34" s="20" t="n">
-        <x:v>1366</x:v>
-      </x:c>
-      <x:c r="BW34" s="21" t="n">
-        <x:v>3.1</x:v>
       </x:c>
     </x:row>
     <x:row r="35" ht="10.2" customHeight="1">
@@ -1503,40 +1503,40 @@
         <x:v>Banks, Savings &amp; Lending Institutions</x:v>
       </x:c>
       <x:c r="J35" s="17" t="n">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="Q35" s="18" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="W35" s="17" t="n">
-        <x:v>261</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="Z35" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AI35" s="17" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="AN35" s="18" t="n">
         <x:v>2.1</x:v>
       </x:c>
       <x:c r="AU35" s="17" t="n">
-        <x:v>385</x:v>
+        <x:v>340</x:v>
       </x:c>
       <x:c r="AY35" s="18" t="n">
-        <x:v>1.8</x:v>
+        <x:v>1.5</x:v>
       </x:c>
       <x:c r="BG35" s="17" t="n">
-        <x:v>28</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="BO35" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.5</x:v>
       </x:c>
       <x:c r="BT35" s="17" t="n">
-        <x:v>173</x:v>
+        <x:v>1023</x:v>
       </x:c>
       <x:c r="BW35" s="18" t="n">
-        <x:v>0.4</x:v>
+        <x:v>2.3</x:v>
       </x:c>
     </x:row>
     <x:row r="36" ht="10.2" customHeight="1">
@@ -1544,37 +1544,37 @@
         <x:v>Securities Brokers</x:v>
       </x:c>
       <x:c r="J36" s="20" t="n">
-        <x:v>23</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="Q36" s="21" t="n">
-        <x:v>1.5</x:v>
+        <x:v>1.7</x:v>
       </x:c>
       <x:c r="W36" s="20" t="n">
-        <x:v>94</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="Z36" s="21" t="n">
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="AI36" s="20" t="n">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="AN36" s="21" t="n">
         <x:v>1.4</x:v>
       </x:c>
       <x:c r="AU36" s="20" t="n">
-        <x:v>111</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="AY36" s="21" t="n">
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="BG36" s="20" t="n">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="BO36" s="21" t="n">
-        <x:v>0.7</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="BT36" s="20" t="n">
-        <x:v>68</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="BW36" s="21" t="n">
         <x:v>0.2</x:v>
@@ -1585,28 +1585,28 @@
         <x:v>Insurance Carriers &amp; Agents</x:v>
       </x:c>
       <x:c r="J37" s="17" t="n">
-        <x:v>34</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="Q37" s="18" t="n">
         <x:v>2.2</x:v>
       </x:c>
       <x:c r="W37" s="17" t="n">
-        <x:v>132</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="Z37" s="18" t="n">
-        <x:v>0.7</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="AI37" s="17" t="n">
-        <x:v>34</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AN37" s="18" t="n">
-        <x:v>1.9</x:v>
+        <x:v>1.6</x:v>
       </x:c>
       <x:c r="AU37" s="17" t="n">
-        <x:v>179</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="AY37" s="18" t="n">
-        <x:v>0.8</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="BG37" s="17" t="n">
         <x:v>25</x:v>
@@ -1615,7 +1615,7 @@
         <x:v>1.1</x:v>
       </x:c>
       <x:c r="BT37" s="17" t="n">
-        <x:v>401</x:v>
+        <x:v>388</x:v>
       </x:c>
       <x:c r="BW37" s="18" t="n">
         <x:v>0.9</x:v>
@@ -1626,37 +1626,37 @@
         <x:v>Real Estate, Holding, Other Investment Offices</x:v>
       </x:c>
       <x:c r="J38" s="20" t="n">
-        <x:v>74</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="Q38" s="21" t="n">
-        <x:v>4.7</x:v>
+        <x:v>4.9</x:v>
       </x:c>
       <x:c r="W38" s="20" t="n">
-        <x:v>519</x:v>
+        <x:v>615</x:v>
       </x:c>
       <x:c r="Z38" s="21" t="n">
-        <x:v>2.6</x:v>
+        <x:v>2.9</x:v>
       </x:c>
       <x:c r="AI38" s="20" t="n">
-        <x:v>95</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="AN38" s="21" t="n">
-        <x:v>5.2</x:v>
+        <x:v>4.9</x:v>
       </x:c>
       <x:c r="AU38" s="20" t="n">
-        <x:v>583</x:v>
+        <x:v>638</x:v>
       </x:c>
       <x:c r="AY38" s="21" t="n">
-        <x:v>2.7</x:v>
+        <x:v>2.9</x:v>
       </x:c>
       <x:c r="BG38" s="20" t="n">
-        <x:v>99</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="BO38" s="21" t="n">
-        <x:v>4.5</x:v>
+        <x:v>4.6</x:v>
       </x:c>
       <x:c r="BT38" s="20" t="n">
-        <x:v>723</x:v>
+        <x:v>761</x:v>
       </x:c>
       <x:c r="BW38" s="21" t="n">
         <x:v>1.7</x:v>
@@ -1682,40 +1682,40 @@
         <x:v>Services Summary</x:v>
       </x:c>
       <x:c r="J40" s="20" t="n">
-        <x:v>697</x:v>
+        <x:v>749</x:v>
       </x:c>
       <x:c r="Q40" s="21" t="n">
+        <x:v>43.6</x:v>
+      </x:c>
+      <x:c r="W40" s="20" t="n">
+        <x:v>12160</x:v>
+      </x:c>
+      <x:c r="Z40" s="21" t="n">
+        <x:v>56.9</x:v>
+      </x:c>
+      <x:c r="AI40" s="20" t="n">
+        <x:v>841</x:v>
+      </x:c>
+      <x:c r="AN40" s="21" t="n">
+        <x:v>44.6</x:v>
+      </x:c>
+      <x:c r="AU40" s="20" t="n">
+        <x:v>9903</x:v>
+      </x:c>
+      <x:c r="AY40" s="21" t="n">
         <x:v>44.4</x:v>
       </x:c>
-      <x:c r="W40" s="20" t="n">
-        <x:v>12126</x:v>
-      </x:c>
-      <x:c r="Z40" s="21" t="n">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="AI40" s="20" t="n">
-        <x:v>820</x:v>
-      </x:c>
-      <x:c r="AN40" s="21" t="n">
-        <x:v>44.7</x:v>
-      </x:c>
-      <x:c r="AU40" s="20" t="n">
-        <x:v>9670</x:v>
-      </x:c>
-      <x:c r="AY40" s="21" t="n">
-        <x:v>44.2</x:v>
-      </x:c>
       <x:c r="BG40" s="20" t="n">
-        <x:v>892</x:v>
+        <x:v>955</x:v>
       </x:c>
       <x:c r="BO40" s="21" t="n">
-        <x:v>40.7</x:v>
+        <x:v>41.1</x:v>
       </x:c>
       <x:c r="BT40" s="20" t="n">
-        <x:v>27713</x:v>
+        <x:v>28101</x:v>
       </x:c>
       <x:c r="BW40" s="21" t="n">
-        <x:v>63.3</x:v>
+        <x:v>62.7</x:v>
       </x:c>
     </x:row>
     <x:row r="41" ht="10.2" customHeight="1">
@@ -1723,37 +1723,37 @@
         <x:v>Hotels &amp; Lodging</x:v>
       </x:c>
       <x:c r="J41" s="17" t="n">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="Q41" s="18" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.7</x:v>
       </x:c>
       <x:c r="W41" s="17" t="n">
-        <x:v>59</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="Z41" s="18" t="n">
         <x:v>0.3</x:v>
       </x:c>
       <x:c r="AI41" s="17" t="n">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="AN41" s="18" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.5</x:v>
       </x:c>
       <x:c r="AU41" s="17" t="n">
-        <x:v>86</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="AY41" s="18" t="n">
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="BG41" s="17" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="BO41" s="18" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="BT41" s="17" t="n">
-        <x:v>214</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="BW41" s="18" t="n">
         <x:v>0.5</x:v>
@@ -1764,37 +1764,37 @@
         <x:v>Automotive Services</x:v>
       </x:c>
       <x:c r="J42" s="20" t="n">
-        <x:v>55</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="Q42" s="21" t="n">
-        <x:v>3.5</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="W42" s="20" t="n">
-        <x:v>284</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="Z42" s="21" t="n">
-        <x:v>1.4</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AI42" s="20" t="n">
-        <x:v>37</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="AN42" s="21" t="n">
-        <x:v>2</x:v>
+        <x:v>2.3</x:v>
       </x:c>
       <x:c r="AU42" s="20" t="n">
-        <x:v>169</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="AY42" s="21" t="n">
-        <x:v>0.8</x:v>
+        <x:v>0.9</x:v>
       </x:c>
       <x:c r="BG42" s="20" t="n">
-        <x:v>98</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="BO42" s="21" t="n">
-        <x:v>4.5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="BT42" s="20" t="n">
-        <x:v>300</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="BW42" s="21" t="n">
         <x:v>0.7</x:v>
@@ -1805,40 +1805,40 @@
         <x:v>Motion Pictures &amp; Amusements</x:v>
       </x:c>
       <x:c r="J43" s="17" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Q43" s="18" t="n">
+        <x:v>2.7</x:v>
+      </x:c>
+      <x:c r="W43" s="17" t="n">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="Z43" s="18" t="n">
+        <x:v>1.4</x:v>
+      </x:c>
+      <x:c r="AI43" s="17" t="n">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AN43" s="18" t="n">
+        <x:v>2.8</x:v>
+      </x:c>
+      <x:c r="AU43" s="17" t="n">
+        <x:v>481</x:v>
+      </x:c>
+      <x:c r="AY43" s="18" t="n">
+        <x:v>2.2</x:v>
+      </x:c>
+      <x:c r="BG43" s="17" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="Q43" s="18" t="n">
-        <x:v>2.5</x:v>
-      </x:c>
-      <x:c r="W43" s="17" t="n">
-        <x:v>234</x:v>
-      </x:c>
-      <x:c r="Z43" s="18" t="n">
-        <x:v>1.2</x:v>
-      </x:c>
-      <x:c r="AI43" s="17" t="n">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="AN43" s="18" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="AU43" s="17" t="n">
-        <x:v>499</x:v>
-      </x:c>
-      <x:c r="AY43" s="18" t="n">
-        <x:v>2.3</x:v>
-      </x:c>
-      <x:c r="BG43" s="17" t="n">
-        <x:v>36</x:v>
-      </x:c>
       <x:c r="BO43" s="18" t="n">
-        <x:v>1.6</x:v>
+        <x:v>1.7</x:v>
       </x:c>
       <x:c r="BT43" s="17" t="n">
-        <x:v>246</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="BW43" s="18" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.7</x:v>
       </x:c>
     </x:row>
     <x:row r="44" ht="10.2" customHeight="1">
@@ -1846,40 +1846,40 @@
         <x:v>Health Services</x:v>
       </x:c>
       <x:c r="J44" s="20" t="n">
-        <x:v>136</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="Q44" s="21" t="n">
-        <x:v>8.7</x:v>
+        <x:v>8.6</x:v>
       </x:c>
       <x:c r="W44" s="20" t="n">
-        <x:v>2499</x:v>
+        <x:v>2300</x:v>
       </x:c>
       <x:c r="Z44" s="21" t="n">
-        <x:v>12.4</x:v>
+        <x:v>10.8</x:v>
       </x:c>
       <x:c r="AI44" s="20" t="n">
-        <x:v>178</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="AN44" s="21" t="n">
-        <x:v>9.7</x:v>
+        <x:v>10.8</x:v>
       </x:c>
       <x:c r="AU44" s="20" t="n">
-        <x:v>3351</x:v>
+        <x:v>3570</x:v>
       </x:c>
       <x:c r="AY44" s="21" t="n">
-        <x:v>15.3</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="BG44" s="20" t="n">
-        <x:v>178</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="BO44" s="21" t="n">
-        <x:v>8.1</x:v>
+        <x:v>8.8</x:v>
       </x:c>
       <x:c r="BT44" s="20" t="n">
-        <x:v>10350</x:v>
+        <x:v>10575</x:v>
       </x:c>
       <x:c r="BW44" s="21" t="n">
-        <x:v>23.7</x:v>
+        <x:v>23.6</x:v>
       </x:c>
     </x:row>
     <x:row r="45" ht="10.2" customHeight="1">
@@ -1887,40 +1887,40 @@
         <x:v>Legal Services</x:v>
       </x:c>
       <x:c r="J45" s="17" t="n">
-        <x:v>44</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="Q45" s="18" t="n">
-        <x:v>2.8</x:v>
+        <x:v>2.4</x:v>
       </x:c>
       <x:c r="W45" s="17" t="n">
-        <x:v>247</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="Z45" s="18" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="AI45" s="17" t="n">
         <x:v>40</x:v>
       </x:c>
       <x:c r="AN45" s="18" t="n">
-        <x:v>2.2</x:v>
+        <x:v>2.1</x:v>
       </x:c>
       <x:c r="AU45" s="17" t="n">
-        <x:v>238</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="AY45" s="18" t="n">
         <x:v>1.1</x:v>
       </x:c>
       <x:c r="BG45" s="17" t="n">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="BO45" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.4</x:v>
       </x:c>
       <x:c r="BT45" s="17" t="n">
-        <x:v>208</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="BW45" s="18" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.6</x:v>
       </x:c>
     </x:row>
     <x:row r="46" ht="10.2" customHeight="1">
@@ -1928,40 +1928,40 @@
         <x:v>Education Institutions &amp; Libraries</x:v>
       </x:c>
       <x:c r="J46" s="20" t="n">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="Q46" s="21" t="n">
         <x:v>1.8</x:v>
       </x:c>
       <x:c r="W46" s="20" t="n">
-        <x:v>545</x:v>
+        <x:v>558</x:v>
       </x:c>
       <x:c r="Z46" s="21" t="n">
-        <x:v>2.7</x:v>
+        <x:v>2.6</x:v>
       </x:c>
       <x:c r="AI46" s="20" t="n">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="AN46" s="21" t="n">
         <x:v>2.4</x:v>
       </x:c>
       <x:c r="AU46" s="20" t="n">
-        <x:v>2022</x:v>
+        <x:v>2050</x:v>
       </x:c>
       <x:c r="AY46" s="21" t="n">
         <x:v>9.2</x:v>
       </x:c>
       <x:c r="BG46" s="20" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="BO46" s="21" t="n">
-        <x:v>3.1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="BT46" s="20" t="n">
-        <x:v>12475</x:v>
+        <x:v>12105</x:v>
       </x:c>
       <x:c r="BW46" s="21" t="n">
-        <x:v>28.5</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="47" ht="10.2" customHeight="1">
@@ -1969,40 +1969,40 @@
         <x:v>Other Services</x:v>
       </x:c>
       <x:c r="J47" s="17" t="n">
-        <x:v>383</x:v>
+        <x:v>418</x:v>
       </x:c>
       <x:c r="Q47" s="18" t="n">
-        <x:v>24.4</x:v>
+        <x:v>24.3</x:v>
       </x:c>
       <x:c r="W47" s="17" t="n">
-        <x:v>8257</x:v>
+        <x:v>8466</x:v>
       </x:c>
       <x:c r="Z47" s="18" t="n">
-        <x:v>40.9</x:v>
+        <x:v>39.6</x:v>
       </x:c>
       <x:c r="AI47" s="17" t="n">
-        <x:v>456</x:v>
+        <x:v>448</x:v>
       </x:c>
       <x:c r="AN47" s="18" t="n">
-        <x:v>24.9</x:v>
+        <x:v>23.7</x:v>
       </x:c>
       <x:c r="AU47" s="17" t="n">
-        <x:v>3305</x:v>
+        <x:v>3274</x:v>
       </x:c>
       <x:c r="AY47" s="18" t="n">
-        <x:v>15.1</x:v>
+        <x:v>14.7</x:v>
       </x:c>
       <x:c r="BG47" s="17" t="n">
-        <x:v>474</x:v>
+        <x:v>503</x:v>
       </x:c>
       <x:c r="BO47" s="18" t="n">
         <x:v>21.6</x:v>
       </x:c>
       <x:c r="BT47" s="17" t="n">
-        <x:v>3920</x:v>
+        <x:v>4341</x:v>
       </x:c>
       <x:c r="BW47" s="18" t="n">
-        <x:v>9</x:v>
+        <x:v>9.7</x:v>
       </x:c>
     </x:row>
     <x:row r="48" ht="9.9" customHeight="1">
@@ -2025,40 +2025,40 @@
         <x:v>Government</x:v>
       </x:c>
       <x:c r="J49" s="17" t="n">
-        <x:v>39</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="Q49" s="18" t="n">
-        <x:v>2.5</x:v>
+        <x:v>2.6</x:v>
       </x:c>
       <x:c r="W49" s="17" t="n">
-        <x:v>987</x:v>
+        <x:v>1228</x:v>
       </x:c>
       <x:c r="Z49" s="18" t="n">
-        <x:v>4.9</x:v>
+        <x:v>5.7</x:v>
       </x:c>
       <x:c r="AI49" s="17" t="n">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="AN49" s="18" t="n">
-        <x:v>0.8</x:v>
+        <x:v>0.9</x:v>
       </x:c>
       <x:c r="AU49" s="17" t="n">
-        <x:v>183</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="AY49" s="18" t="n">
-        <x:v>0.8</x:v>
+        <x:v>1.1</x:v>
       </x:c>
       <x:c r="BG49" s="17" t="n">
-        <x:v>46</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="BO49" s="18" t="n">
-        <x:v>2.1</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="BT49" s="17" t="n">
-        <x:v>1110</x:v>
+        <x:v>1189</x:v>
       </x:c>
       <x:c r="BW49" s="18" t="n">
-        <x:v>2.5</x:v>
+        <x:v>2.7</x:v>
       </x:c>
     </x:row>
     <x:row r="50" ht="9.9" customHeight="1">
@@ -2081,40 +2081,40 @@
         <x:v>Unclassified Establishments </x:v>
       </x:c>
       <x:c r="J51" s="17" t="n">
-        <x:v>134</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="Q51" s="18" t="n">
-        <x:v>8.5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="W51" s="17" t="n">
-        <x:v>62</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="Z51" s="18" t="n">
         <x:v>0.3</x:v>
       </x:c>
       <x:c r="AI51" s="17" t="n">
-        <x:v>180</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="AN51" s="18" t="n">
-        <x:v>9.8</x:v>
+        <x:v>10.9</x:v>
       </x:c>
       <x:c r="AU51" s="17" t="n">
-        <x:v>69</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="AY51" s="18" t="n">
-        <x:v>0.3</x:v>
+        <x:v>0.4</x:v>
       </x:c>
       <x:c r="BG51" s="17" t="n">
-        <x:v>220</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="BO51" s="18" t="n">
-        <x:v>10</x:v>
+        <x:v>10.2</x:v>
       </x:c>
       <x:c r="BT51" s="17" t="n">
-        <x:v>187</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="BW51" s="18" t="n">
-        <x:v>0.4</x:v>
+        <x:v>0.1</x:v>
       </x:c>
     </x:row>
     <x:row r="52" ht="9.9" customHeight="1">
@@ -2137,37 +2137,37 @@
         <x:v>Totals</x:v>
       </x:c>
       <x:c r="J53" s="17" t="n">
-        <x:v>1569</x:v>
+        <x:v>1718</x:v>
       </x:c>
       <x:c r="Q53" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="W53" s="17" t="n">
-        <x:v>20210</x:v>
+        <x:v>21383</x:v>
       </x:c>
       <x:c r="Z53" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="AI53" s="17" t="n">
-        <x:v>1833</x:v>
+        <x:v>1887</x:v>
       </x:c>
       <x:c r="AN53" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="AU53" s="17" t="n">
-        <x:v>21860</x:v>
+        <x:v>22285</x:v>
       </x:c>
       <x:c r="AY53" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="BG53" s="17" t="n">
-        <x:v>2190</x:v>
+        <x:v>2326</x:v>
       </x:c>
       <x:c r="BO53" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="BT53" s="17" t="n">
-        <x:v>43758</x:v>
+        <x:v>44836</x:v>
       </x:c>
       <x:c r="BW53" s="22" t="str">
         <x:v>100.0%</x:v>
@@ -2198,7 +2198,7 @@
       <x:c r="C59" s="28"/>
       <x:c r="D59" s="1"/>
       <x:c r="O59" s="3" t="str">
-        <x:v>August 27, 2021</x:v>
+        <x:v>June 30, 2022</x:v>
       </x:c>
     </x:row>
     <x:row r="60" ht="11.75" customHeight="1">
@@ -2209,7 +2209,7 @@
     </x:row>
     <x:row r="61" ht="15" customHeight="1">
       <x:c r="C61" s="32" t="str">
-        <x:v>©2021 Esri</x:v>
+        <x:v>©2022 Esri</x:v>
       </x:c>
       <x:c r="D61" s="1"/>
       <x:c r="O61" s="31"/>
@@ -2334,37 +2334,37 @@
         <x:v>Agriculture, Forestry, Fishing &amp; Hunting</x:v>
       </x:c>
       <x:c r="J72" s="17" t="n">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="Q72" s="18" t="n">
-        <x:v>0.1</x:v>
+        <x:v>0.2</x:v>
       </x:c>
       <x:c r="W72" s="17" t="n">
-        <x:v>13</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="Z72" s="18" t="n">
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="AJ72" s="17" t="n">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="AO72" s="18" t="n">
-        <x:v>0.2</x:v>
+        <x:v>0.1</x:v>
       </x:c>
       <x:c r="AV72" s="17" t="n">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="AZ72" s="18" t="n">
-        <x:v>0.1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="BI72" s="17" t="n">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="BO72" s="18" t="n">
-        <x:v>0.4</x:v>
+        <x:v>0.3</x:v>
       </x:c>
       <x:c r="BT72" s="17" t="n">
-        <x:v>49</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="BW72" s="18" t="n">
         <x:v>0.1</x:v>
@@ -2375,28 +2375,28 @@
         <x:v>Mining</x:v>
       </x:c>
       <x:c r="J73" s="20" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="Q73" s="21" t="n">
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="W73" s="20" t="n">
-        <x:v>6</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="Z73" s="21" t="n">
-        <x:v>0</x:v>
+        <x:v>0.2</x:v>
       </x:c>
       <x:c r="AJ73" s="20" t="n">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="AO73" s="21" t="n">
-        <x:v>0</x:v>
+        <x:v>0.1</x:v>
       </x:c>
       <x:c r="AV73" s="20" t="n">
-        <x:v>2</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="AZ73" s="21" t="n">
-        <x:v>0</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="BI73" s="20" t="n">
         <x:v>1</x:v>
@@ -2405,7 +2405,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="BT73" s="20" t="n">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="BW73" s="21" t="n">
         <x:v>0.1</x:v>
@@ -2419,10 +2419,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="Q74" s="18" t="n">
-        <x:v>0.3</x:v>
+        <x:v>0.2</x:v>
       </x:c>
       <x:c r="W74" s="17" t="n">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="Z74" s="18" t="n">
         <x:v>0.2</x:v>
@@ -2434,7 +2434,7 @@
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="AV74" s="17" t="n">
-        <x:v>96</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="AZ74" s="18" t="n">
         <x:v>0.4</x:v>
@@ -2446,10 +2446,10 @@
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="BT74" s="17" t="n">
-        <x:v>270</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="BW74" s="18" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.3</x:v>
       </x:c>
     </x:row>
     <x:row r="75" ht="10.2" customHeight="1">
@@ -2457,37 +2457,37 @@
         <x:v>Construction</x:v>
       </x:c>
       <x:c r="J75" s="20" t="n">
-        <x:v>85</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="Q75" s="21" t="n">
-        <x:v>5.4</x:v>
+        <x:v>5.2</x:v>
       </x:c>
       <x:c r="W75" s="20" t="n">
-        <x:v>633</x:v>
+        <x:v>493</x:v>
       </x:c>
       <x:c r="Z75" s="21" t="n">
-        <x:v>3.1</x:v>
+        <x:v>2.3</x:v>
       </x:c>
       <x:c r="AJ75" s="20" t="n">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="AO75" s="21" t="n">
         <x:v>6.3</x:v>
       </x:c>
       <x:c r="AV75" s="20" t="n">
-        <x:v>755</x:v>
+        <x:v>642</x:v>
       </x:c>
       <x:c r="AZ75" s="21" t="n">
-        <x:v>3.5</x:v>
+        <x:v>2.9</x:v>
       </x:c>
       <x:c r="BI75" s="20" t="n">
-        <x:v>171</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="BO75" s="21" t="n">
-        <x:v>7.8</x:v>
+        <x:v>7.9</x:v>
       </x:c>
       <x:c r="BT75" s="20" t="n">
-        <x:v>1269</x:v>
+        <x:v>1309</x:v>
       </x:c>
       <x:c r="BW75" s="21" t="n">
         <x:v>2.9</x:v>
@@ -2498,40 +2498,40 @@
         <x:v>Manufacturing</x:v>
       </x:c>
       <x:c r="J76" s="17" t="n">
-        <x:v>39</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="Q76" s="18" t="n">
         <x:v>2.5</x:v>
       </x:c>
       <x:c r="W76" s="17" t="n">
-        <x:v>366</x:v>
+        <x:v>451</x:v>
       </x:c>
       <x:c r="Z76" s="18" t="n">
-        <x:v>1.8</x:v>
+        <x:v>2.1</x:v>
       </x:c>
       <x:c r="AJ76" s="17" t="n">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="AO76" s="18" t="n">
         <x:v>2.5</x:v>
       </x:c>
       <x:c r="AV76" s="17" t="n">
-        <x:v>585</x:v>
+        <x:v>731</x:v>
       </x:c>
       <x:c r="AZ76" s="18" t="n">
-        <x:v>2.7</x:v>
+        <x:v>3.3</x:v>
       </x:c>
       <x:c r="BI76" s="17" t="n">
         <x:v>81</x:v>
       </x:c>
       <x:c r="BO76" s="18" t="n">
-        <x:v>3.7</x:v>
+        <x:v>3.5</x:v>
       </x:c>
       <x:c r="BT76" s="17" t="n">
-        <x:v>1608</x:v>
+        <x:v>1550</x:v>
       </x:c>
       <x:c r="BW76" s="18" t="n">
-        <x:v>3.7</x:v>
+        <x:v>3.5</x:v>
       </x:c>
     </x:row>
     <x:row r="77" ht="10.2" customHeight="1">
@@ -2539,40 +2539,40 @@
         <x:v>Wholesale Trade</x:v>
       </x:c>
       <x:c r="J77" s="20" t="n">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="Q77" s="21" t="n">
-        <x:v>2</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="W77" s="20" t="n">
-        <x:v>323</x:v>
+        <x:v>569</x:v>
       </x:c>
       <x:c r="Z77" s="21" t="n">
-        <x:v>1.6</x:v>
+        <x:v>2.7</x:v>
       </x:c>
       <x:c r="AJ77" s="20" t="n">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="AO77" s="21" t="n">
         <x:v>1.7</x:v>
       </x:c>
       <x:c r="AV77" s="20" t="n">
-        <x:v>430</x:v>
+        <x:v>482</x:v>
       </x:c>
       <x:c r="AZ77" s="21" t="n">
-        <x:v>2</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="BI77" s="20" t="n">
-        <x:v>76</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="BO77" s="21" t="n">
-        <x:v>3.5</x:v>
+        <x:v>3.4</x:v>
       </x:c>
       <x:c r="BT77" s="20" t="n">
-        <x:v>1295</x:v>
+        <x:v>1144</x:v>
       </x:c>
       <x:c r="BW77" s="21" t="n">
-        <x:v>3</x:v>
+        <x:v>2.6</x:v>
       </x:c>
     </x:row>
     <x:row r="78" ht="10.2" customHeight="1">
@@ -2580,40 +2580,40 @@
         <x:v>Retail Trade</x:v>
       </x:c>
       <x:c r="J78" s="17" t="n">
-        <x:v>203</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="Q78" s="18" t="n">
+        <x:v>12.6</x:v>
+      </x:c>
+      <x:c r="W78" s="17" t="n">
+        <x:v>3162</x:v>
+      </x:c>
+      <x:c r="Z78" s="18" t="n">
+        <x:v>14.8</x:v>
+      </x:c>
+      <x:c r="AJ78" s="17" t="n">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="AO78" s="18" t="n">
+        <x:v>11.7</x:v>
+      </x:c>
+      <x:c r="AV78" s="17" t="n">
+        <x:v>5875</x:v>
+      </x:c>
+      <x:c r="AZ78" s="18" t="n">
+        <x:v>26.4</x:v>
+      </x:c>
+      <x:c r="BI78" s="17" t="n">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="BO78" s="18" t="n">
+        <x:v>12.3</x:v>
+      </x:c>
+      <x:c r="BT78" s="17" t="n">
+        <x:v>5764</x:v>
+      </x:c>
+      <x:c r="BW78" s="18" t="n">
         <x:v>12.9</x:v>
-      </x:c>
-      <x:c r="W78" s="17" t="n">
-        <x:v>2823</x:v>
-      </x:c>
-      <x:c r="Z78" s="18" t="n">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="AJ78" s="17" t="n">
-        <x:v>227</x:v>
-      </x:c>
-      <x:c r="AO78" s="18" t="n">
-        <x:v>12.4</x:v>
-      </x:c>
-      <x:c r="AV78" s="17" t="n">
-        <x:v>6135</x:v>
-      </x:c>
-      <x:c r="AZ78" s="18" t="n">
-        <x:v>28.1</x:v>
-      </x:c>
-      <x:c r="BI78" s="17" t="n">
-        <x:v>291</x:v>
-      </x:c>
-      <x:c r="BO78" s="18" t="n">
-        <x:v>13.3</x:v>
-      </x:c>
-      <x:c r="BT78" s="17" t="n">
-        <x:v>5697</x:v>
-      </x:c>
-      <x:c r="BW78" s="18" t="n">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="79" ht="10.2" customHeight="1">
@@ -2624,37 +2624,37 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="Q79" s="21" t="n">
-        <x:v>1.7</x:v>
+        <x:v>1.5</x:v>
       </x:c>
       <x:c r="W79" s="20" t="n">
-        <x:v>512</x:v>
+        <x:v>580</x:v>
       </x:c>
       <x:c r="Z79" s="21" t="n">
-        <x:v>2.5</x:v>
+        <x:v>2.7</x:v>
       </x:c>
       <x:c r="AJ79" s="20" t="n">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="AO79" s="21" t="n">
-        <x:v>1</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="AV79" s="20" t="n">
-        <x:v>371</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="AZ79" s="21" t="n">
-        <x:v>1.7</x:v>
+        <x:v>1.4</x:v>
       </x:c>
       <x:c r="BI79" s="20" t="n">
-        <x:v>49</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="BO79" s="21" t="n">
-        <x:v>2.2</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="BT79" s="20" t="n">
-        <x:v>488</x:v>
+        <x:v>713</x:v>
       </x:c>
       <x:c r="BW79" s="21" t="n">
-        <x:v>1.1</x:v>
+        <x:v>1.6</x:v>
       </x:c>
     </x:row>
     <x:row r="80" ht="10.2" customHeight="1">
@@ -2662,28 +2662,28 @@
         <x:v>Furniture &amp; Home Furnishings Stores</x:v>
       </x:c>
       <x:c r="J80" s="17" t="n">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="Q80" s="18" t="n">
-        <x:v>0.8</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="W80" s="17" t="n">
-        <x:v>84</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="Z80" s="18" t="n">
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="AJ80" s="17" t="n">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="AO80" s="18" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AV80" s="17" t="n">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="AZ80" s="18" t="n">
         <x:v>0.9</x:v>
-      </x:c>
-      <x:c r="AV80" s="17" t="n">
-        <x:v>215</x:v>
-      </x:c>
-      <x:c r="AZ80" s="18" t="n">
-        <x:v>1</x:v>
       </x:c>
       <x:c r="BI80" s="17" t="n">
         <x:v>11</x:v>
@@ -2692,10 +2692,10 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="BT80" s="17" t="n">
-        <x:v>107</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="BW80" s="18" t="n">
-        <x:v>0.2</x:v>
+        <x:v>0.1</x:v>
       </x:c>
     </x:row>
     <x:row r="81" ht="10.2" customHeight="1">
@@ -2703,37 +2703,37 @@
         <x:v>Electronics &amp; Appliance Stores</x:v>
       </x:c>
       <x:c r="J81" s="20" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="Q81" s="21" t="n">
         <x:v>0.3</x:v>
       </x:c>
       <x:c r="W81" s="20" t="n">
-        <x:v>11</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="Z81" s="21" t="n">
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="AJ81" s="20" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="AO81" s="21" t="n">
-        <x:v>0.3</x:v>
+        <x:v>0.2</x:v>
       </x:c>
       <x:c r="AV81" s="20" t="n">
-        <x:v>15</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="AZ81" s="21" t="n">
-        <x:v>0.1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="BI81" s="20" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="BO81" s="21" t="n">
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="BT81" s="20" t="n">
-        <x:v>150</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="BW81" s="21" t="n">
         <x:v>0.3</x:v>
@@ -2744,40 +2744,40 @@
         <x:v>Bldg Material &amp; Garden Equipment &amp; Supplies Dealers</x:v>
       </x:c>
       <x:c r="J82" s="17" t="n">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="Q82" s="18" t="n">
         <x:v>0.9</x:v>
       </x:c>
       <x:c r="W82" s="17" t="n">
-        <x:v>490</x:v>
+        <x:v>418</x:v>
       </x:c>
       <x:c r="Z82" s="18" t="n">
-        <x:v>2.4</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="AJ82" s="17" t="n">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="AO82" s="18" t="n">
         <x:v>0.8</x:v>
       </x:c>
       <x:c r="AV82" s="17" t="n">
-        <x:v>409</x:v>
+        <x:v>484</x:v>
       </x:c>
       <x:c r="AZ82" s="18" t="n">
-        <x:v>1.9</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="BI82" s="17" t="n">
-        <x:v>33</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="BO82" s="18" t="n">
-        <x:v>1.5</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="BT82" s="17" t="n">
-        <x:v>585</x:v>
+        <x:v>497</x:v>
       </x:c>
       <x:c r="BW82" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.1</x:v>
       </x:c>
     </x:row>
     <x:row r="83" ht="10.2" customHeight="1">
@@ -2785,40 +2785,40 @@
         <x:v>Food &amp; Beverage Stores</x:v>
       </x:c>
       <x:c r="J83" s="20" t="n">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="Q83" s="21" t="n">
         <x:v>1.8</x:v>
       </x:c>
       <x:c r="W83" s="20" t="n">
-        <x:v>480</x:v>
+        <x:v>512</x:v>
       </x:c>
       <x:c r="Z83" s="21" t="n">
         <x:v>2.4</x:v>
       </x:c>
       <x:c r="AJ83" s="20" t="n">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="AO83" s="21" t="n">
-        <x:v>2</x:v>
+        <x:v>1.9</x:v>
       </x:c>
       <x:c r="AV83" s="20" t="n">
-        <x:v>791</x:v>
+        <x:v>808</x:v>
       </x:c>
       <x:c r="AZ83" s="21" t="n">
         <x:v>3.6</x:v>
       </x:c>
       <x:c r="BI83" s="20" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="BO83" s="21" t="n">
-        <x:v>2.4</x:v>
+        <x:v>2.3</x:v>
       </x:c>
       <x:c r="BT83" s="20" t="n">
-        <x:v>553</x:v>
+        <x:v>729</x:v>
       </x:c>
       <x:c r="BW83" s="21" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.6</x:v>
       </x:c>
     </x:row>
     <x:row r="84" ht="10.2" customHeight="1">
@@ -2826,40 +2826,40 @@
         <x:v>Health &amp; Personal Care Stores</x:v>
       </x:c>
       <x:c r="J84" s="17" t="n">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="Q84" s="18" t="n">
+        <x:v>0.9</x:v>
+      </x:c>
+      <x:c r="W84" s="17" t="n">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="Z84" s="18" t="n">
+        <x:v>0.7</x:v>
+      </x:c>
+      <x:c r="AJ84" s="17" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="AO84" s="18" t="n">
+        <x:v>2.1</x:v>
+      </x:c>
+      <x:c r="AV84" s="17" t="n">
+        <x:v>438</x:v>
+      </x:c>
+      <x:c r="AZ84" s="18" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="BI84" s="17" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="BO84" s="18" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="W84" s="17" t="n">
-        <x:v>116</x:v>
-      </x:c>
-      <x:c r="Z84" s="18" t="n">
-        <x:v>0.6</x:v>
-      </x:c>
-      <x:c r="AJ84" s="17" t="n">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="AO84" s="18" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="AV84" s="17" t="n">
-        <x:v>422</x:v>
-      </x:c>
-      <x:c r="AZ84" s="18" t="n">
-        <x:v>1.9</x:v>
-      </x:c>
-      <x:c r="BI84" s="17" t="n">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="BO84" s="18" t="n">
-        <x:v>1.2</x:v>
-      </x:c>
       <x:c r="BT84" s="17" t="n">
-        <x:v>207</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="BW84" s="18" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.4</x:v>
       </x:c>
     </x:row>
     <x:row r="85" ht="10.2" customHeight="1">
@@ -2867,19 +2867,19 @@
         <x:v>Gasoline Stations</x:v>
       </x:c>
       <x:c r="J85" s="20" t="n">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="Q85" s="21" t="n">
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="W85" s="20" t="n">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="Z85" s="21" t="n">
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="AJ85" s="20" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="AO85" s="21" t="n">
         <x:v>0.4</x:v>
@@ -2894,10 +2894,10 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="BO85" s="21" t="n">
-        <x:v>1.1</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="BT85" s="20" t="n">
-        <x:v>128</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="BW85" s="21" t="n">
         <x:v>0.3</x:v>
@@ -2908,40 +2908,40 @@
         <x:v>Clothing &amp; Clothing Accessories Stores</x:v>
       </x:c>
       <x:c r="J86" s="17" t="n">
-        <x:v>31</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="Q86" s="18" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="W86" s="17" t="n">
-        <x:v>173</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="Z86" s="18" t="n">
+        <x:v>0.8</x:v>
+      </x:c>
+      <x:c r="AJ86" s="17" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="AO86" s="18" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AV86" s="17" t="n">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="AZ86" s="18" t="n">
         <x:v>0.9</x:v>
       </x:c>
-      <x:c r="AJ86" s="17" t="n">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="AO86" s="18" t="n">
-        <x:v>1.3</x:v>
-      </x:c>
-      <x:c r="AV86" s="17" t="n">
-        <x:v>299</x:v>
-      </x:c>
-      <x:c r="AZ86" s="18" t="n">
-        <x:v>1.4</x:v>
-      </x:c>
       <x:c r="BI86" s="17" t="n">
-        <x:v>12</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="BO86" s="18" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.4</x:v>
       </x:c>
       <x:c r="BT86" s="17" t="n">
-        <x:v>75</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="BW86" s="18" t="n">
-        <x:v>0.2</x:v>
+        <x:v>0.1</x:v>
       </x:c>
     </x:row>
     <x:row r="87" ht="10.2" customHeight="1">
@@ -2949,37 +2949,37 @@
         <x:v>Sport Goods, Hobby, Book, &amp; Music Stores</x:v>
       </x:c>
       <x:c r="J87" s="20" t="n">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="Q87" s="21" t="n">
         <x:v>1.1</x:v>
       </x:c>
       <x:c r="W87" s="20" t="n">
-        <x:v>109</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="Z87" s="21" t="n">
+        <x:v>0.6</x:v>
+      </x:c>
+      <x:c r="AJ87" s="20" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="AO87" s="21" t="n">
+        <x:v>0.8</x:v>
+      </x:c>
+      <x:c r="AV87" s="20" t="n">
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="AZ87" s="21" t="n">
+        <x:v>0.8</x:v>
+      </x:c>
+      <x:c r="BI87" s="20" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="BO87" s="21" t="n">
         <x:v>0.5</x:v>
       </x:c>
-      <x:c r="AJ87" s="20" t="n">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="AO87" s="21" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AV87" s="20" t="n">
-        <x:v>199</x:v>
-      </x:c>
-      <x:c r="AZ87" s="21" t="n">
-        <x:v>0.9</x:v>
-      </x:c>
-      <x:c r="BI87" s="20" t="n">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="BO87" s="21" t="n">
-        <x:v>0.6</x:v>
-      </x:c>
       <x:c r="BT87" s="20" t="n">
-        <x:v>77</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="BW87" s="21" t="n">
         <x:v>0.2</x:v>
@@ -2990,28 +2990,28 @@
         <x:v>General Merchandise Stores</x:v>
       </x:c>
       <x:c r="J88" s="17" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="Q88" s="18" t="n">
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="W88" s="17" t="n">
-        <x:v>128</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="Z88" s="18" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="AJ88" s="17" t="n">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="AO88" s="18" t="n">
-        <x:v>1</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="AV88" s="17" t="n">
-        <x:v>762</x:v>
+        <x:v>711</x:v>
       </x:c>
       <x:c r="AZ88" s="18" t="n">
-        <x:v>3.5</x:v>
+        <x:v>3.2</x:v>
       </x:c>
       <x:c r="BI88" s="17" t="n">
         <x:v>13</x:v>
@@ -3020,10 +3020,10 @@
         <x:v>0.6</x:v>
       </x:c>
       <x:c r="BT88" s="17" t="n">
-        <x:v>797</x:v>
+        <x:v>767</x:v>
       </x:c>
       <x:c r="BW88" s="18" t="n">
-        <x:v>1.8</x:v>
+        <x:v>1.7</x:v>
       </x:c>
     </x:row>
     <x:row r="89" ht="10.2" customHeight="1">
@@ -3031,40 +3031,40 @@
         <x:v>Miscellaneous Store Retailers</x:v>
       </x:c>
       <x:c r="J89" s="20" t="n">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="Q89" s="21" t="n">
-        <x:v>2.5</x:v>
+        <x:v>2.4</x:v>
       </x:c>
       <x:c r="W89" s="20" t="n">
-        <x:v>325</x:v>
+        <x:v>365</x:v>
       </x:c>
       <x:c r="Z89" s="21" t="n">
-        <x:v>1.6</x:v>
+        <x:v>1.7</x:v>
       </x:c>
       <x:c r="AJ89" s="20" t="n">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="AO89" s="21" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AV89" s="20" t="n">
-        <x:v>346</x:v>
+        <x:v>370</x:v>
       </x:c>
       <x:c r="AZ89" s="21" t="n">
-        <x:v>1.6</x:v>
+        <x:v>1.7</x:v>
       </x:c>
       <x:c r="BI89" s="20" t="n">
         <x:v>36</x:v>
       </x:c>
       <x:c r="BO89" s="21" t="n">
-        <x:v>1.6</x:v>
+        <x:v>1.5</x:v>
       </x:c>
       <x:c r="BT89" s="20" t="n">
-        <x:v>339</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="BW89" s="21" t="n">
-        <x:v>0.8</x:v>
+        <x:v>0.7</x:v>
       </x:c>
     </x:row>
     <x:row r="90" ht="10.2" customHeight="1">
@@ -3078,34 +3078,34 @@
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="W90" s="17" t="n">
-        <x:v>365</x:v>
+        <x:v>507</x:v>
       </x:c>
       <x:c r="Z90" s="18" t="n">
-        <x:v>1.8</x:v>
+        <x:v>2.4</x:v>
       </x:c>
       <x:c r="AJ90" s="17" t="n">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="AO90" s="18" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="AV90" s="17" t="n">
-        <x:v>2266</x:v>
+        <x:v>2124</x:v>
       </x:c>
       <x:c r="AZ90" s="18" t="n">
-        <x:v>10.4</x:v>
+        <x:v>9.5</x:v>
       </x:c>
       <x:c r="BI90" s="17" t="n">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="BO90" s="18" t="n">
         <x:v>0.7</x:v>
       </x:c>
       <x:c r="BT90" s="17" t="n">
-        <x:v>2192</x:v>
+        <x:v>2052</x:v>
       </x:c>
       <x:c r="BW90" s="18" t="n">
-        <x:v>5</x:v>
+        <x:v>4.6</x:v>
       </x:c>
     </x:row>
     <x:row r="91" ht="10.2" customHeight="1">
@@ -3113,40 +3113,40 @@
         <x:v>Transportation &amp; Warehousing</x:v>
       </x:c>
       <x:c r="J91" s="20" t="n">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="Q91" s="21" t="n">
+        <x:v>1.2</x:v>
+      </x:c>
+      <x:c r="W91" s="20" t="n">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="Z91" s="21" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="W91" s="20" t="n">
-        <x:v>152</x:v>
-      </x:c>
-      <x:c r="Z91" s="21" t="n">
-        <x:v>0.8</x:v>
-      </x:c>
       <x:c r="AJ91" s="20" t="n">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="AO91" s="21" t="n">
-        <x:v>1.7</x:v>
+        <x:v>1.9</x:v>
       </x:c>
       <x:c r="AV91" s="20" t="n">
-        <x:v>249</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="AZ91" s="21" t="n">
-        <x:v>1.1</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="BI91" s="20" t="n">
-        <x:v>57</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="BO91" s="21" t="n">
-        <x:v>2.6</x:v>
+        <x:v>2.8</x:v>
       </x:c>
       <x:c r="BT91" s="20" t="n">
         <x:v>507</x:v>
       </x:c>
       <x:c r="BW91" s="21" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1.1</x:v>
       </x:c>
     </x:row>
     <x:row r="92" ht="10.2" customHeight="1">
@@ -3154,37 +3154,37 @@
         <x:v>Information</x:v>
       </x:c>
       <x:c r="J92" s="17" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="Q92" s="18" t="n">
         <x:v>1.5</x:v>
       </x:c>
       <x:c r="W92" s="17" t="n">
-        <x:v>195</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="Z92" s="18" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="AJ92" s="17" t="n">
-        <x:v>36</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="AO92" s="18" t="n">
-        <x:v>2</x:v>
+        <x:v>1.7</x:v>
       </x:c>
       <x:c r="AV92" s="17" t="n">
-        <x:v>445</x:v>
+        <x:v>424</x:v>
       </x:c>
       <x:c r="AZ92" s="18" t="n">
-        <x:v>2</x:v>
+        <x:v>1.9</x:v>
       </x:c>
       <x:c r="BI92" s="17" t="n">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="BO92" s="18" t="n">
         <x:v>1.2</x:v>
       </x:c>
       <x:c r="BT92" s="17" t="n">
-        <x:v>369</x:v>
+        <x:v>376</x:v>
       </x:c>
       <x:c r="BW92" s="18" t="n">
         <x:v>0.8</x:v>
@@ -3195,40 +3195,40 @@
         <x:v>Finance &amp; Insurance</x:v>
       </x:c>
       <x:c r="J93" s="20" t="n">
-        <x:v>90</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="Q93" s="21" t="n">
-        <x:v>5.7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="W93" s="20" t="n">
-        <x:v>492</x:v>
+        <x:v>497</x:v>
       </x:c>
       <x:c r="Z93" s="21" t="n">
-        <x:v>2.4</x:v>
+        <x:v>2.3</x:v>
       </x:c>
       <x:c r="AJ93" s="20" t="n">
-        <x:v>98</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="AO93" s="21" t="n">
-        <x:v>5.3</x:v>
+        <x:v>5.1</x:v>
       </x:c>
       <x:c r="AV93" s="20" t="n">
-        <x:v>677</x:v>
+        <x:v>589</x:v>
       </x:c>
       <x:c r="AZ93" s="21" t="n">
-        <x:v>3.1</x:v>
+        <x:v>2.6</x:v>
       </x:c>
       <x:c r="BI93" s="20" t="n">
-        <x:v>70</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="BO93" s="21" t="n">
-        <x:v>3.2</x:v>
+        <x:v>3.4</x:v>
       </x:c>
       <x:c r="BT93" s="20" t="n">
-        <x:v>645</x:v>
+        <x:v>1489</x:v>
       </x:c>
       <x:c r="BW93" s="21" t="n">
-        <x:v>1.5</x:v>
+        <x:v>3.3</x:v>
       </x:c>
     </x:row>
     <x:row r="94" ht="10.2" customHeight="1">
@@ -3236,40 +3236,40 @@
         <x:v>Central Bank/Credit Intermediation &amp; Related Activities</x:v>
       </x:c>
       <x:c r="J94" s="17" t="n">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="Q94" s="18" t="n">
-        <x:v>2</x:v>
+        <x:v>1.9</x:v>
       </x:c>
       <x:c r="W94" s="17" t="n">
-        <x:v>262</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="Z94" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AJ94" s="17" t="n">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="AO94" s="18" t="n">
-        <x:v>2</x:v>
+        <x:v>1.9</x:v>
       </x:c>
       <x:c r="AV94" s="17" t="n">
-        <x:v>378</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="AZ94" s="18" t="n">
-        <x:v>1.7</x:v>
+        <x:v>1.4</x:v>
       </x:c>
       <x:c r="BI94" s="17" t="n">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="BO94" s="18" t="n">
         <x:v>1.3</x:v>
       </x:c>
       <x:c r="BT94" s="17" t="n">
-        <x:v>173</x:v>
+        <x:v>1018</x:v>
       </x:c>
       <x:c r="BW94" s="18" t="n">
-        <x:v>0.4</x:v>
+        <x:v>2.3</x:v>
       </x:c>
     </x:row>
     <x:row r="95" ht="10.2" customHeight="1">
@@ -3277,37 +3277,37 @@
         <x:v>Securities, Commodity Contracts &amp; Other Financial Investments &amp; Other Related Activities</x:v>
       </x:c>
       <x:c r="J95" s="20" t="n">
-        <x:v>24</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="Q95" s="21" t="n">
-        <x:v>1.5</x:v>
+        <x:v>1.9</x:v>
       </x:c>
       <x:c r="W95" s="20" t="n">
-        <x:v>98</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="Z95" s="21" t="n">
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="AJ95" s="20" t="n">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="AO95" s="21" t="n">
-        <x:v>1.5</x:v>
+        <x:v>1.6</x:v>
       </x:c>
       <x:c r="AV95" s="20" t="n">
-        <x:v>119</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="AZ95" s="21" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="BI95" s="20" t="n">
-        <x:v>16</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="BO95" s="21" t="n">
-        <x:v>0.7</x:v>
+        <x:v>0.9</x:v>
       </x:c>
       <x:c r="BT95" s="20" t="n">
-        <x:v>69</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="BW95" s="21" t="n">
         <x:v>0.2</x:v>
@@ -3318,37 +3318,37 @@
         <x:v>Insurance Carriers &amp; Related Activities; Funds, Trusts &amp; Other Financial Vehicles</x:v>
       </x:c>
       <x:c r="J96" s="17" t="n">
-        <x:v>34</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="Q96" s="18" t="n">
         <x:v>2.2</x:v>
       </x:c>
       <x:c r="W96" s="17" t="n">
-        <x:v>132</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="Z96" s="18" t="n">
-        <x:v>0.7</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="AJ96" s="17" t="n">
-        <x:v>34</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AO96" s="18" t="n">
-        <x:v>1.9</x:v>
+        <x:v>1.6</x:v>
       </x:c>
       <x:c r="AV96" s="17" t="n">
-        <x:v>179</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="AZ96" s="18" t="n">
-        <x:v>0.8</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="BI96" s="17" t="n">
         <x:v>26</x:v>
       </x:c>
       <x:c r="BO96" s="18" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1.1</x:v>
       </x:c>
       <x:c r="BT96" s="17" t="n">
-        <x:v>403</x:v>
+        <x:v>390</x:v>
       </x:c>
       <x:c r="BW96" s="18" t="n">
         <x:v>0.9</x:v>
@@ -3359,37 +3359,37 @@
         <x:v>Real Estate, Rental &amp; Leasing</x:v>
       </x:c>
       <x:c r="J97" s="20" t="n">
-        <x:v>86</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="Q97" s="21" t="n">
         <x:v>5.5</x:v>
       </x:c>
       <x:c r="W97" s="20" t="n">
-        <x:v>532</x:v>
+        <x:v>626</x:v>
       </x:c>
       <x:c r="Z97" s="21" t="n">
-        <x:v>2.6</x:v>
+        <x:v>2.9</x:v>
       </x:c>
       <x:c r="AJ97" s="20" t="n">
-        <x:v>108</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="AO97" s="21" t="n">
-        <x:v>5.9</x:v>
+        <x:v>5.7</x:v>
       </x:c>
       <x:c r="AV97" s="20" t="n">
-        <x:v>586</x:v>
+        <x:v>643</x:v>
       </x:c>
       <x:c r="AZ97" s="21" t="n">
-        <x:v>2.7</x:v>
+        <x:v>2.9</x:v>
       </x:c>
       <x:c r="BI97" s="20" t="n">
-        <x:v>114</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="BO97" s="21" t="n">
         <x:v>5.2</x:v>
       </x:c>
       <x:c r="BT97" s="20" t="n">
-        <x:v>617</x:v>
+        <x:v>639</x:v>
       </x:c>
       <x:c r="BW97" s="21" t="n">
         <x:v>1.4</x:v>
@@ -3400,40 +3400,40 @@
         <x:v>Professional, Scientific &amp; Tech Services</x:v>
       </x:c>
       <x:c r="J98" s="17" t="n">
-        <x:v>172</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="Q98" s="18" t="n">
-        <x:v>11</x:v>
+        <x:v>10.8</x:v>
       </x:c>
       <x:c r="W98" s="17" t="n">
-        <x:v>6539</x:v>
+        <x:v>6525</x:v>
       </x:c>
       <x:c r="Z98" s="18" t="n">
-        <x:v>32.4</x:v>
+        <x:v>30.5</x:v>
       </x:c>
       <x:c r="AJ98" s="17" t="n">
-        <x:v>194</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="AO98" s="18" t="n">
-        <x:v>10.6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="AV98" s="17" t="n">
-        <x:v>1262</x:v>
+        <x:v>1168</x:v>
       </x:c>
       <x:c r="AZ98" s="18" t="n">
-        <x:v>5.8</x:v>
+        <x:v>5.2</x:v>
       </x:c>
       <x:c r="BI98" s="17" t="n">
-        <x:v>190</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="BO98" s="18" t="n">
         <x:v>8.7</x:v>
       </x:c>
       <x:c r="BT98" s="17" t="n">
-        <x:v>1549</x:v>
+        <x:v>1714</x:v>
       </x:c>
       <x:c r="BW98" s="18" t="n">
-        <x:v>3.5</x:v>
+        <x:v>3.8</x:v>
       </x:c>
     </x:row>
     <x:row r="99" ht="10.2" customHeight="1">
@@ -3441,40 +3441,40 @@
         <x:v>Legal Services</x:v>
       </x:c>
       <x:c r="J99" s="20" t="n">
-        <x:v>47</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="Q99" s="21" t="n">
-        <x:v>3</x:v>
+        <x:v>2.6</x:v>
       </x:c>
       <x:c r="W99" s="20" t="n">
-        <x:v>263</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="Z99" s="21" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="AJ99" s="20" t="n">
         <x:v>44</x:v>
       </x:c>
       <x:c r="AO99" s="21" t="n">
-        <x:v>2.4</x:v>
+        <x:v>2.3</x:v>
       </x:c>
       <x:c r="AV99" s="20" t="n">
-        <x:v>258</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="AZ99" s="21" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1.1</x:v>
       </x:c>
       <x:c r="BI99" s="20" t="n">
-        <x:v>33</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="BO99" s="21" t="n">
-        <x:v>1.5</x:v>
+        <x:v>1.6</x:v>
       </x:c>
       <x:c r="BT99" s="20" t="n">
-        <x:v>379</x:v>
+        <x:v>490</x:v>
       </x:c>
       <x:c r="BW99" s="21" t="n">
-        <x:v>0.9</x:v>
+        <x:v>1.1</x:v>
       </x:c>
     </x:row>
     <x:row r="100" ht="10.2" customHeight="1">
@@ -3482,13 +3482,13 @@
         <x:v>Management of Companies &amp; Enterprises</x:v>
       </x:c>
       <x:c r="J100" s="17" t="n">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="Q100" s="18" t="n">
-        <x:v>0.1</x:v>
+        <x:v>0.2</x:v>
       </x:c>
       <x:c r="W100" s="17" t="n">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="Z100" s="18" t="n">
         <x:v>0</x:v>
@@ -3506,13 +3506,13 @@
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="BI100" s="17" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="BO100" s="18" t="n">
         <x:v>0.3</x:v>
       </x:c>
       <x:c r="BT100" s="17" t="n">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="BW100" s="18" t="n">
         <x:v>0</x:v>
@@ -3523,40 +3523,40 @@
         <x:v>Administrative &amp; Support &amp; Waste Management &amp; Remediation Services</x:v>
       </x:c>
       <x:c r="J101" s="20" t="n">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="Q101" s="21" t="n">
-        <x:v>3.3</x:v>
+        <x:v>3.1</x:v>
       </x:c>
       <x:c r="W101" s="20" t="n">
-        <x:v>256</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="Z101" s="21" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AJ101" s="20" t="n">
-        <x:v>66</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="AO101" s="21" t="n">
-        <x:v>3.6</x:v>
+        <x:v>3.8</x:v>
       </x:c>
       <x:c r="AV101" s="20" t="n">
-        <x:v>285</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="AZ101" s="21" t="n">
         <x:v>1.3</x:v>
       </x:c>
       <x:c r="BI101" s="20" t="n">
-        <x:v>74</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="BO101" s="21" t="n">
-        <x:v>3.4</x:v>
+        <x:v>3.5</x:v>
       </x:c>
       <x:c r="BT101" s="20" t="n">
-        <x:v>529</x:v>
+        <x:v>511</x:v>
       </x:c>
       <x:c r="BW101" s="21" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1.1</x:v>
       </x:c>
     </x:row>
     <x:row r="102" ht="10.2" customHeight="1">
@@ -3564,40 +3564,40 @@
         <x:v>Educational Services</x:v>
       </x:c>
       <x:c r="J102" s="17" t="n">
-        <x:v>38</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="Q102" s="18" t="n">
-        <x:v>2.4</x:v>
+        <x:v>2.6</x:v>
       </x:c>
       <x:c r="W102" s="17" t="n">
-        <x:v>586</x:v>
+        <x:v>589</x:v>
       </x:c>
       <x:c r="Z102" s="18" t="n">
-        <x:v>2.9</x:v>
+        <x:v>2.8</x:v>
       </x:c>
       <x:c r="AJ102" s="17" t="n">
         <x:v>53</x:v>
       </x:c>
       <x:c r="AO102" s="18" t="n">
-        <x:v>2.9</x:v>
+        <x:v>2.8</x:v>
       </x:c>
       <x:c r="AV102" s="17" t="n">
-        <x:v>2067</x:v>
+        <x:v>2090</x:v>
       </x:c>
       <x:c r="AZ102" s="18" t="n">
-        <x:v>9.5</x:v>
+        <x:v>9.4</x:v>
       </x:c>
       <x:c r="BI102" s="17" t="n">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="BO102" s="18" t="n">
-        <x:v>3.2</x:v>
+        <x:v>3.1</x:v>
       </x:c>
       <x:c r="BT102" s="17" t="n">
-        <x:v>12283</x:v>
+        <x:v>11914</x:v>
       </x:c>
       <x:c r="BW102" s="18" t="n">
-        <x:v>28.1</x:v>
+        <x:v>26.6</x:v>
       </x:c>
     </x:row>
     <x:row r="103" ht="10.2" customHeight="1">
@@ -3605,37 +3605,37 @@
         <x:v>Health Care &amp; Social Assistance</x:v>
       </x:c>
       <x:c r="J103" s="20" t="n">
-        <x:v>166</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="Q103" s="21" t="n">
         <x:v>10.6</x:v>
       </x:c>
       <x:c r="W103" s="20" t="n">
-        <x:v>3028</x:v>
+        <x:v>2912</x:v>
       </x:c>
       <x:c r="Z103" s="21" t="n">
-        <x:v>15</x:v>
+        <x:v>13.6</x:v>
       </x:c>
       <x:c r="AJ103" s="20" t="n">
-        <x:v>228</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="AO103" s="21" t="n">
-        <x:v>12.4</x:v>
+        <x:v>13.4</x:v>
       </x:c>
       <x:c r="AV103" s="20" t="n">
-        <x:v>4166</x:v>
+        <x:v>4587</x:v>
       </x:c>
       <x:c r="AZ103" s="21" t="n">
-        <x:v>19.1</x:v>
+        <x:v>20.6</x:v>
       </x:c>
       <x:c r="BI103" s="20" t="n">
-        <x:v>232</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="BO103" s="21" t="n">
-        <x:v>10.6</x:v>
+        <x:v>11.4</x:v>
       </x:c>
       <x:c r="BT103" s="20" t="n">
-        <x:v>11571</x:v>
+        <x:v>11841</x:v>
       </x:c>
       <x:c r="BW103" s="21" t="n">
         <x:v>26.4</x:v>
@@ -3646,40 +3646,40 @@
         <x:v>Arts, Entertainment &amp; Recreation</x:v>
       </x:c>
       <x:c r="J104" s="17" t="n">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="Q104" s="18" t="n">
         <x:v>1.7</x:v>
       </x:c>
       <x:c r="W104" s="17" t="n">
-        <x:v>214</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="Z104" s="18" t="n">
-        <x:v>1.1</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AJ104" s="17" t="n">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="AO104" s="18" t="n">
         <x:v>2.3</x:v>
       </x:c>
       <x:c r="AV104" s="17" t="n">
-        <x:v>467</x:v>
+        <x:v>442</x:v>
       </x:c>
       <x:c r="AZ104" s="18" t="n">
-        <x:v>2.1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="BI104" s="17" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="BO104" s="18" t="n">
-        <x:v>1.3</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="BT104" s="17" t="n">
-        <x:v>234</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="BW104" s="18" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.6</x:v>
       </x:c>
     </x:row>
     <x:row r="105" ht="10.2" customHeight="1">
@@ -3687,40 +3687,40 @@
         <x:v>Accommodation &amp; Food Services</x:v>
       </x:c>
       <x:c r="J105" s="20" t="n">
-        <x:v>135</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="Q105" s="21" t="n">
-        <x:v>8.6</x:v>
+        <x:v>8.8</x:v>
       </x:c>
       <x:c r="W105" s="20" t="n">
-        <x:v>1597</x:v>
+        <x:v>1669</x:v>
       </x:c>
       <x:c r="Z105" s="21" t="n">
-        <x:v>7.9</x:v>
+        <x:v>7.8</x:v>
       </x:c>
       <x:c r="AJ105" s="20" t="n">
-        <x:v>138</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="AO105" s="21" t="n">
         <x:v>7.5</x:v>
       </x:c>
       <x:c r="AV105" s="20" t="n">
-        <x:v>2047</x:v>
+        <x:v>1993</x:v>
       </x:c>
       <x:c r="AZ105" s="21" t="n">
-        <x:v>9.4</x:v>
+        <x:v>8.9</x:v>
       </x:c>
       <x:c r="BI105" s="20" t="n">
-        <x:v>154</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="BO105" s="21" t="n">
-        <x:v>7</x:v>
+        <x:v>7.4</x:v>
       </x:c>
       <x:c r="BT105" s="20" t="n">
-        <x:v>2659</x:v>
+        <x:v>2765</x:v>
       </x:c>
       <x:c r="BW105" s="21" t="n">
-        <x:v>6.1</x:v>
+        <x:v>6.2</x:v>
       </x:c>
     </x:row>
     <x:row r="106" ht="10.2" customHeight="1">
@@ -3728,37 +3728,37 @@
         <x:v>Accommodation</x:v>
       </x:c>
       <x:c r="J106" s="17" t="n">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="Q106" s="18" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.7</x:v>
       </x:c>
       <x:c r="W106" s="17" t="n">
-        <x:v>59</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="Z106" s="18" t="n">
         <x:v>0.3</x:v>
       </x:c>
       <x:c r="AJ106" s="17" t="n">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="AO106" s="18" t="n">
-        <x:v>0.6</x:v>
+        <x:v>0.5</x:v>
       </x:c>
       <x:c r="AV106" s="17" t="n">
-        <x:v>86</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="AZ106" s="18" t="n">
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="BI106" s="17" t="n">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="BO106" s="18" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0.6</x:v>
       </x:c>
       <x:c r="BT106" s="17" t="n">
-        <x:v>214</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="BW106" s="18" t="n">
         <x:v>0.5</x:v>
@@ -3769,40 +3769,40 @@
         <x:v>Food Services &amp; Drinking Places</x:v>
       </x:c>
       <x:c r="J107" s="20" t="n">
-        <x:v>125</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="Q107" s="21" t="n">
-        <x:v>8</x:v>
+        <x:v>8.1</x:v>
       </x:c>
       <x:c r="W107" s="20" t="n">
-        <x:v>1538</x:v>
+        <x:v>1601</x:v>
       </x:c>
       <x:c r="Z107" s="21" t="n">
-        <x:v>7.6</x:v>
+        <x:v>7.5</x:v>
       </x:c>
       <x:c r="AJ107" s="20" t="n">
-        <x:v>127</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="AO107" s="21" t="n">
         <x:v>6.9</x:v>
       </x:c>
       <x:c r="AV107" s="20" t="n">
-        <x:v>1961</x:v>
+        <x:v>1909</x:v>
       </x:c>
       <x:c r="AZ107" s="21" t="n">
-        <x:v>9</x:v>
+        <x:v>8.6</x:v>
       </x:c>
       <x:c r="BI107" s="20" t="n">
-        <x:v>143</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="BO107" s="21" t="n">
-        <x:v>6.5</x:v>
+        <x:v>6.8</x:v>
       </x:c>
       <x:c r="BT107" s="20" t="n">
-        <x:v>2445</x:v>
+        <x:v>2554</x:v>
       </x:c>
       <x:c r="BW107" s="21" t="n">
-        <x:v>5.6</x:v>
+        <x:v>5.7</x:v>
       </x:c>
     </x:row>
     <x:row r="108" ht="10.2" customHeight="1">
@@ -3810,40 +3810,40 @@
         <x:v>Other Services (except Public Administration)</x:v>
       </x:c>
       <x:c r="J108" s="17" t="n">
-        <x:v>221</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="Q108" s="18" t="n">
-        <x:v>14.1</x:v>
+        <x:v>13.6</x:v>
       </x:c>
       <x:c r="W108" s="17" t="n">
-        <x:v>1355</x:v>
+        <x:v>1531</x:v>
       </x:c>
       <x:c r="Z108" s="18" t="n">
-        <x:v>6.7</x:v>
+        <x:v>7.2</x:v>
       </x:c>
       <x:c r="AJ108" s="17" t="n">
-        <x:v>216</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="AO108" s="18" t="n">
+        <x:v>11.6</x:v>
+      </x:c>
+      <x:c r="AV108" s="17" t="n">
+        <x:v>1473</x:v>
+      </x:c>
+      <x:c r="AZ108" s="18" t="n">
+        <x:v>6.6</x:v>
+      </x:c>
+      <x:c r="BI108" s="17" t="n">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="BO108" s="18" t="n">
         <x:v>11.8</x:v>
       </x:c>
-      <x:c r="AV108" s="17" t="n">
-        <x:v>1330</x:v>
-      </x:c>
-      <x:c r="AZ108" s="18" t="n">
-        <x:v>6.1</x:v>
-      </x:c>
-      <x:c r="BI108" s="17" t="n">
-        <x:v>269</x:v>
-      </x:c>
-      <x:c r="BO108" s="18" t="n">
-        <x:v>12.3</x:v>
-      </x:c>
       <x:c r="BT108" s="17" t="n">
-        <x:v>1242</x:v>
+        <x:v>1554</x:v>
       </x:c>
       <x:c r="BW108" s="18" t="n">
-        <x:v>2.8</x:v>
+        <x:v>3.5</x:v>
       </x:c>
     </x:row>
     <x:row r="109" ht="10.2" customHeight="1">
@@ -3851,34 +3851,34 @@
         <x:v>Automotive Repair &amp; Maintenance</x:v>
       </x:c>
       <x:c r="J109" s="20" t="n">
-        <x:v>46</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="Q109" s="21" t="n">
-        <x:v>2.9</x:v>
+        <x:v>2.5</x:v>
       </x:c>
       <x:c r="W109" s="20" t="n">
-        <x:v>240</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="Z109" s="21" t="n">
-        <x:v>1.2</x:v>
+        <x:v>1.1</x:v>
       </x:c>
       <x:c r="AJ109" s="20" t="n">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="AO109" s="21" t="n">
-        <x:v>1.7</x:v>
+        <x:v>1.9</x:v>
       </x:c>
       <x:c r="AV109" s="20" t="n">
-        <x:v>146</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="AZ109" s="21" t="n">
-        <x:v>0.7</x:v>
+        <x:v>0.8</x:v>
       </x:c>
       <x:c r="BI109" s="20" t="n">
-        <x:v>82</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="BO109" s="21" t="n">
-        <x:v>3.7</x:v>
+        <x:v>3.4</x:v>
       </x:c>
       <x:c r="BT109" s="20" t="n">
         <x:v>210</x:v>
@@ -3892,40 +3892,40 @@
         <x:v>Public Administration</x:v>
       </x:c>
       <x:c r="J110" s="17" t="n">
-        <x:v>39</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="Q110" s="18" t="n">
-        <x:v>2.5</x:v>
+        <x:v>2.6</x:v>
       </x:c>
       <x:c r="W110" s="17" t="n">
-        <x:v>987</x:v>
+        <x:v>1228</x:v>
       </x:c>
       <x:c r="Z110" s="18" t="n">
-        <x:v>4.9</x:v>
+        <x:v>5.7</x:v>
       </x:c>
       <x:c r="AJ110" s="17" t="n">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="AO110" s="18" t="n">
-        <x:v>0.8</x:v>
+        <x:v>0.9</x:v>
       </x:c>
       <x:c r="AV110" s="17" t="n">
-        <x:v>183</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="AZ110" s="18" t="n">
-        <x:v>0.8</x:v>
+        <x:v>1.1</x:v>
       </x:c>
       <x:c r="BI110" s="17" t="n">
-        <x:v>46</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="BO110" s="18" t="n">
-        <x:v>2.1</x:v>
+        <x:v>2.2</x:v>
       </x:c>
       <x:c r="BT110" s="17" t="n">
-        <x:v>1110</x:v>
+        <x:v>1189</x:v>
       </x:c>
       <x:c r="BW110" s="18" t="n">
-        <x:v>2.5</x:v>
+        <x:v>2.7</x:v>
       </x:c>
     </x:row>
     <x:row r="111" ht="9.9" customHeight="1">
@@ -3948,40 +3948,40 @@
         <x:v>Unclassified Establishments </x:v>
       </x:c>
       <x:c r="J112" s="17" t="n">
-        <x:v>133</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="Q112" s="18" t="n">
-        <x:v>8.5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="W112" s="17" t="n">
-        <x:v>59</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="Z112" s="18" t="n">
-        <x:v>0.3</x:v>
+        <x:v>0.2</x:v>
       </x:c>
       <x:c r="AJ112" s="17" t="n">
-        <x:v>179</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="AO112" s="18" t="n">
-        <x:v>9.8</x:v>
+        <x:v>10.9</x:v>
       </x:c>
       <x:c r="AV112" s="17" t="n">
-        <x:v>67</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="AZ112" s="18" t="n">
-        <x:v>0.3</x:v>
+        <x:v>0.4</x:v>
       </x:c>
       <x:c r="BI112" s="17" t="n">
-        <x:v>219</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="BO112" s="18" t="n">
-        <x:v>10</x:v>
+        <x:v>10.1</x:v>
       </x:c>
       <x:c r="BT112" s="17" t="n">
-        <x:v>183</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="BW112" s="18" t="n">
-        <x:v>0.4</x:v>
+        <x:v>0.1</x:v>
       </x:c>
     </x:row>
     <x:row r="113" ht="9.9" customHeight="1">
@@ -4004,37 +4004,37 @@
         <x:v>Total</x:v>
       </x:c>
       <x:c r="J114" s="17" t="n">
-        <x:v>1569</x:v>
+        <x:v>1718</x:v>
       </x:c>
       <x:c r="Q114" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="W114" s="17" t="n">
-        <x:v>20210</x:v>
+        <x:v>21383</x:v>
       </x:c>
       <x:c r="Z114" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="AJ114" s="17" t="n">
-        <x:v>1833</x:v>
+        <x:v>1887</x:v>
       </x:c>
       <x:c r="AO114" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="AV114" s="17" t="n">
-        <x:v>21860</x:v>
+        <x:v>22285</x:v>
       </x:c>
       <x:c r="AZ114" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="BI114" s="17" t="n">
-        <x:v>2190</x:v>
+        <x:v>2326</x:v>
       </x:c>
       <x:c r="BO114" s="22" t="str">
         <x:v>100.0%</x:v>
       </x:c>
       <x:c r="BT114" s="17" t="n">
-        <x:v>43758</x:v>
+        <x:v>44836</x:v>
       </x:c>
       <x:c r="BW114" s="22" t="str">
         <x:v>100.0%</x:v>
@@ -4065,7 +4065,7 @@
       <x:c r="C120" s="28"/>
       <x:c r="D120" s="1"/>
       <x:c r="O120" s="3" t="str">
-        <x:v>August 27, 2021</x:v>
+        <x:v>June 30, 2022</x:v>
       </x:c>
     </x:row>
     <x:row r="121" ht="11.75" customHeight="1">
@@ -4076,7 +4076,7 @@
     </x:row>
     <x:row r="122" ht="15" customHeight="1">
       <x:c r="C122" s="32" t="str">
-        <x:v>©2021 Esri</x:v>
+        <x:v>©2022 Esri</x:v>
       </x:c>
       <x:c r="D122" s="1"/>
       <x:c r="O122" s="31"/>

</xml_diff>